<commit_message>
updates to the dlb modules
</commit_message>
<xml_diff>
--- a/wetb/dlb/tests/test_files/IEC64100-1_DLB_DTU_ref.xlsx
+++ b/wetb/dlb/tests/test_files/IEC64100-1_DLB_DTU_ref.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mmpe\programming\python\WindEnergyToolbox\wetb\dlb\tests\test_files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="18150" windowHeight="6375"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="18150" windowHeight="6375" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DLC" sheetId="1" r:id="rId1"/>
     <sheet name="Sensors" sheetId="3" r:id="rId2"/>
     <sheet name="Variables" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -108,9 +113,6 @@
     <t>MxBR</t>
   </si>
   <si>
-    <t>(26,32,38)</t>
-  </si>
-  <si>
     <t>PyBT</t>
   </si>
   <si>
@@ -361,12 +363,15 @@
   </si>
   <si>
     <t>Hub height [m]</t>
+  </si>
+  <si>
+    <t>(26,29,32)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0E+00"/>
   </numFmts>
@@ -614,6 +619,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -661,7 +669,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -696,7 +704,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -908,7 +916,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -933,19 +941,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H1" s="21" t="s">
         <v>3</v>
@@ -960,16 +968,16 @@
         <v>6</v>
       </c>
       <c r="L1" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="N1" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="N1" s="21" t="s">
-        <v>82</v>
-      </c>
       <c r="O1" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P1" s="21" t="s">
         <v>7</v>
@@ -977,48 +985,48 @@
     </row>
     <row r="2" spans="1:16" s="27" customFormat="1" ht="48.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F2" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="H2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:16" s="28" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1026,16 +1034,16 @@
         <v>11</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3" s="31" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F3" s="33" t="s">
         <v>18</v>
@@ -1047,7 +1055,7 @@
         <v>2</v>
       </c>
       <c r="I3" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J3" s="31" t="s">
         <v>10</v>
@@ -1059,7 +1067,7 @@
         <v>97.5</v>
       </c>
       <c r="M3" s="31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N3" s="31" t="s">
         <v>19</v>
@@ -1082,10 +1090,10 @@
         <v>14</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F4" s="33" t="s">
         <v>18</v>
@@ -1097,7 +1105,7 @@
         <v>2</v>
       </c>
       <c r="I4" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J4" s="31" t="s">
         <v>10</v>
@@ -1117,7 +1125,7 @@
     </row>
     <row r="5" spans="1:16" s="28" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>8</v>
@@ -1126,10 +1134,10 @@
         <v>14</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F5" s="33">
         <v>0</v>
@@ -1141,10 +1149,10 @@
         <v>10</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K5" s="31" t="s">
         <v>10</v>
@@ -1161,7 +1169,7 @@
     </row>
     <row r="6" spans="1:16" s="28" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B6" s="31" t="s">
         <v>8</v>
@@ -1170,10 +1178,10 @@
         <v>14</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F6" s="33">
         <v>0</v>
@@ -1185,7 +1193,7 @@
         <v>10</v>
       </c>
       <c r="I6" s="31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J6" s="31" t="s">
         <v>10</v>
@@ -1233,7 +1241,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -1243,8 +1251,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1263,31 +1271,31 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>37</v>
-      </c>
       <c r="E1" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="J1" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1295,20 +1303,20 @@
         <v>26</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="14">
         <v>17</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H2" s="9">
         <v>4</v>
@@ -1330,14 +1338,14 @@
         <v>18</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H3" s="9">
         <v>4</v>
@@ -1356,17 +1364,17 @@
         <v>24</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>30</v>
+        <v>113</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H4" s="9">
         <v>10</v>
@@ -1379,20 +1387,20 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="8"/>
@@ -1402,19 +1410,19 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="D6" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>98</v>
-      </c>
       <c r="E6" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
@@ -1425,19 +1433,19 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="C7" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="D7" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>47</v>
-      </c>
       <c r="E7" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
@@ -1448,11 +1456,11 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
@@ -1465,22 +1473,22 @@
         <v>1</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K8" s="8"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>88</v>
-      </c>
       <c r="D9" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
@@ -1494,16 +1502,16 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>91</v>
-      </c>
       <c r="D10" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -1521,7 +1529,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -1532,7 +1540,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A11" sqref="A11:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1559,7 +1567,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1570,7 +1578,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1581,12 +1589,12 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1594,35 +1602,35 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" t="s">
         <v>101</v>
       </c>
-      <c r="B6" t="s">
-        <v>102</v>
-      </c>
       <c r="C6" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7">
         <v>121</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B8">
         <v>90</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1630,46 +1638,46 @@
         <v>16</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10">
         <v>46</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="19" t="s">
         <v>57</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="19" t="s">
         <v>61</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>